<commit_message>
commit cahier des charges + cahier de recette
</commit_message>
<xml_diff>
--- a/documentation/GANTT.xlsx
+++ b/documentation/GANTT.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leduc\Desktop\TP-N-1-PHPMySQL-SN2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\projetgps\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0DD4B0-E3F6-4536-9A0E-527BC9B35061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3717706-6FFE-474F-AA52-EC6B54D45A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>ACTIVITY</t>
   </si>
   <si>
-    <t>Activity 10</t>
-  </si>
-  <si>
     <t>Activity 11</t>
   </si>
   <si>
@@ -214,9 +211,6 @@
     <t>Créer une page pour afficher la position et la vitesse de l'utilisateur</t>
   </si>
   <si>
-    <t>Faire la design du site</t>
-  </si>
-  <si>
     <t>Use case</t>
   </si>
   <si>
@@ -233,6 +227,12 @@
   </si>
   <si>
     <t>Faire la bdd</t>
+  </si>
+  <si>
+    <t>Faire le design du site</t>
+  </si>
+  <si>
+    <t>Créer la page pour les administrateurs</t>
   </si>
 </sst>
 </file>
@@ -1043,8 +1043,8 @@
   </sheetPr>
   <dimension ref="B1:BO30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1068,21 +1068,21 @@
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
       <c r="F2" s="24"/>
       <c r="G2" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H2" s="11">
         <v>9</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L2" s="31"/>
       <c r="M2" s="31"/>
@@ -1090,21 +1090,21 @@
       <c r="O2" s="32"/>
       <c r="P2" s="13"/>
       <c r="Q2" s="30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R2" s="33"/>
       <c r="S2" s="33"/>
       <c r="T2" s="32"/>
       <c r="U2" s="14"/>
       <c r="V2" s="22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="W2" s="23"/>
       <c r="X2" s="23"/>
       <c r="Y2" s="34"/>
       <c r="Z2" s="15"/>
       <c r="AA2" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AB2" s="23"/>
       <c r="AC2" s="23"/>
@@ -1114,7 +1114,7 @@
       <c r="AG2" s="34"/>
       <c r="AH2" s="16"/>
       <c r="AI2" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AJ2" s="23"/>
       <c r="AK2" s="23"/>
@@ -1129,22 +1129,22 @@
         <v>1</v>
       </c>
       <c r="C3" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="E3" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="F3" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="G3" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="29" t="s">
-        <v>27</v>
-      </c>
       <c r="H3" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
@@ -1260,53 +1260,53 @@
     </row>
     <row r="5" spans="2:67" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="18">
         <v>1</v>
       </c>
       <c r="D5" s="18">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E5" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="18">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G5" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:67" ht="99" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C6" s="18">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D6" s="18">
+        <v>5</v>
+      </c>
+      <c r="E6" s="18">
         <v>6</v>
       </c>
-      <c r="E6" s="18">
-        <v>0</v>
-      </c>
       <c r="F6" s="18">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G6" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:67" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C7" s="18">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D7" s="18">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E7" s="18">
         <v>0</v>
@@ -1320,7 +1320,7 @@
     </row>
     <row r="8" spans="2:67" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C8" s="18">
         <v>1</v>
@@ -1340,7 +1340,7 @@
     </row>
     <row r="9" spans="2:67" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C9" s="18">
         <v>3</v>
@@ -1360,7 +1360,7 @@
     </row>
     <row r="10" spans="2:67" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C10" s="18">
         <v>5</v>
@@ -1380,7 +1380,7 @@
     </row>
     <row r="11" spans="2:67" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C11" s="18">
         <v>8</v>
@@ -1400,7 +1400,7 @@
     </row>
     <row r="12" spans="2:67" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C12" s="18">
         <v>11</v>
@@ -1420,7 +1420,7 @@
     </row>
     <row r="13" spans="2:67" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C13" s="18">
         <v>1</v>
@@ -1429,30 +1429,30 @@
         <v>3</v>
       </c>
       <c r="E13" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="18">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G13" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:67" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="18">
+        <v>11</v>
+      </c>
+      <c r="D14" s="18">
         <v>2</v>
       </c>
-      <c r="C14" s="18">
-        <v>6</v>
-      </c>
-      <c r="D14" s="18">
-        <v>5</v>
-      </c>
       <c r="E14" s="18">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F14" s="18">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G14" s="19">
         <v>1</v>
@@ -1460,7 +1460,7 @@
     </row>
     <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15" s="21">
         <v>6</v>
@@ -1480,7 +1480,7 @@
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16" s="18">
         <v>9</v>
@@ -1500,7 +1500,7 @@
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="18">
         <v>9</v>
@@ -1520,7 +1520,7 @@
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" s="18">
         <v>9</v>
@@ -1540,7 +1540,7 @@
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" s="18">
         <v>9</v>
@@ -1560,7 +1560,7 @@
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20" s="18">
         <v>10</v>
@@ -1580,7 +1580,7 @@
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C21" s="18">
         <v>11</v>
@@ -1600,7 +1600,7 @@
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" s="18">
         <v>12</v>
@@ -1620,7 +1620,7 @@
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C23" s="18">
         <v>12</v>
@@ -1640,7 +1640,7 @@
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C24" s="18">
         <v>14</v>
@@ -1660,7 +1660,7 @@
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C25" s="18">
         <v>14</v>
@@ -1680,7 +1680,7 @@
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C26" s="18">
         <v>14</v>
@@ -1700,7 +1700,7 @@
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C27" s="18">
         <v>15</v>
@@ -1720,7 +1720,7 @@
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C28" s="18">
         <v>15</v>
@@ -1740,7 +1740,7 @@
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C29" s="18">
         <v>15</v>
@@ -1760,7 +1760,7 @@
     </row>
     <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C30" s="18">
         <v>16</v>

</xml_diff>